<commit_message>
add 10 tests to factorial
</commit_message>
<xml_diff>
--- a/classwork_1/module_4_practice_1.xlsx
+++ b/classwork_1/module_4_practice_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krish\Desktop\1\module_testing\classwork_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEFC9369-EA6C-4507-B97B-A8E4ADECB64F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9D78959-6918-4F4F-88EA-B9518941B5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{0861009E-620E-42F4-A7CE-5A21C66E0B2F}"/>
+    <workbookView xWindow="11820" yWindow="276" windowWidth="11304" windowHeight="11772" xr2:uid="{0861009E-620E-42F4-A7CE-5A21C66E0B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Калькулятор" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="44">
   <si>
     <t>Идентификатор теста</t>
   </si>
@@ -104,21 +104,6 @@
     <t>ТС-015</t>
   </si>
   <si>
-    <t>ТС-016</t>
-  </si>
-  <si>
-    <t>ТС-017</t>
-  </si>
-  <si>
-    <t>ТС-018</t>
-  </si>
-  <si>
-    <t>ТС-019</t>
-  </si>
-  <si>
-    <t>ТС-020</t>
-  </si>
-  <si>
     <t>Фактический результат</t>
   </si>
   <si>
@@ -131,67 +116,58 @@
     <t>PASSED</t>
   </si>
   <si>
-    <t>Проверка работы с положительными целыми числами</t>
-  </si>
-  <si>
-    <t>AssertionError</t>
-  </si>
-  <si>
-    <t>Корректность работы операции сложения</t>
-  </si>
-  <si>
-    <t>Корректность работы операции вычитания</t>
-  </si>
-  <si>
-    <t>Корректность работы операции деления</t>
-  </si>
-  <si>
     <t>Корректность работы операции умножения</t>
   </si>
   <si>
-    <t>Проверка работы операции с отрицательными числами</t>
-  </si>
-  <si>
-    <t>Обработка строки</t>
-  </si>
-  <si>
-    <t>Проверка работы с большим и малым числом</t>
-  </si>
-  <si>
-    <t>Проверка работы с нулевым значением</t>
-  </si>
-  <si>
-    <t>5, 5</t>
-  </si>
-  <si>
-    <t>Вызвать функцию и передать положительные числа</t>
-  </si>
-  <si>
-    <t>-5, -5</t>
-  </si>
-  <si>
-    <t>Вызвать функцию и передать отрицательные числа</t>
-  </si>
-  <si>
-    <t>"5", "5"</t>
-  </si>
-  <si>
-    <t>Вызвать функцию и передать строковое значение</t>
-  </si>
-  <si>
-    <t>5, 50000</t>
-  </si>
-  <si>
-    <t>Вызвать функцию и передать малое и большое число</t>
-  </si>
-  <si>
-    <t>5, 0</t>
-  </si>
-  <si>
-    <t>Вызвать функцию и передать нулевое значение</t>
-  </si>
-  <si>
-    <t>ZeroDivisionError</t>
+    <t>Корректность работы операции суммирования</t>
+  </si>
+  <si>
+    <t>Корректность работы операции вычисления среднего значения</t>
+  </si>
+  <si>
+    <t>Проверка работы с отрицательными числами</t>
+  </si>
+  <si>
+    <t>Проверка работы с положительными числами</t>
+  </si>
+  <si>
+    <t>Проверка работы с положительными и отрицательными числами</t>
+  </si>
+  <si>
+    <t>Проверка работы с нулевыми числами</t>
+  </si>
+  <si>
+    <t>Проверка работы со значениями имеющими различные типы данных</t>
+  </si>
+  <si>
+    <t>[1, 2, 3]</t>
+  </si>
+  <si>
+    <t>[-1, -2, -3]</t>
+  </si>
+  <si>
+    <t>[-1, 2, -3]</t>
+  </si>
+  <si>
+    <t>[0, 0, 0]</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с положительными числами</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с отрицательными числами</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с положительными и отрицательными числами</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список с нулевыми числами</t>
+  </si>
+  <si>
+    <t>["1", 2, 3.0]</t>
+  </si>
+  <si>
+    <t>Вызвать функцию и передать список со значениями с различными типами данных</t>
   </si>
 </sst>
 </file>
@@ -199,7 +175,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -330,7 +306,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="170" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -652,16 +628,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16EF1CFD-9705-4AB0-BC95-161102859BA4}">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="44" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8:G27"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="44" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="A22" activeCellId="1" sqref="A17 A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="60" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="16.44140625" customWidth="1"/>
-    <col min="2" max="2" width="44" customWidth="1"/>
+    <col min="2" max="2" width="48.33203125" customWidth="1"/>
     <col min="3" max="3" width="42.77734375" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" style="5" customWidth="1"/>
     <col min="5" max="5" width="48.5546875" customWidth="1"/>
@@ -675,23 +651,21 @@
     </row>
     <row r="2" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="7" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="7" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>35</v>
-      </c>
+      <c r="B5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="40.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="7"/>
@@ -716,10 +690,10 @@
         <v>5</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -727,25 +701,23 @@
         <v>6</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F8" s="12">
-        <v>10</v>
-      </c>
-      <c r="G8" s="12">
-        <v>10</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G8" s="12"/>
       <c r="H8" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -753,51 +725,47 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F9" s="12">
-        <v>-10</v>
-      </c>
-      <c r="G9" s="12">
-        <v>-10</v>
-      </c>
+        <v>-6</v>
+      </c>
+      <c r="G9" s="12"/>
       <c r="H9" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>32</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F10" s="12">
+        <v>-2</v>
+      </c>
+      <c r="G10" s="12"/>
       <c r="H10" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -805,51 +773,47 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="12">
+        <v>0</v>
+      </c>
+      <c r="G11" s="12"/>
+      <c r="H11" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F11" s="12">
-        <v>50005</v>
-      </c>
-      <c r="G11" s="12">
-        <v>50005</v>
-      </c>
-      <c r="H11" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>40</v>
-      </c>
       <c r="D12" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="12">
-        <v>5</v>
-      </c>
-      <c r="G12" s="12">
-        <v>5</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G12" s="12"/>
       <c r="H12" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -857,25 +821,23 @@
         <v>12</v>
       </c>
       <c r="B13" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="E13" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F13" s="12">
-        <v>0</v>
-      </c>
-      <c r="G13" s="12">
-        <v>0</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="G13" s="12"/>
       <c r="H13" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -883,51 +845,47 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F14" s="12">
-        <v>0</v>
-      </c>
-      <c r="G14" s="12">
-        <v>0</v>
-      </c>
+        <v>-6</v>
+      </c>
+      <c r="G14" s="12"/>
       <c r="H14" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>32</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F15" s="12">
+        <v>6</v>
+      </c>
+      <c r="G15" s="12"/>
       <c r="H15" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -935,51 +893,47 @@
         <v>15</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F16" s="12">
-        <v>-49995</v>
-      </c>
-      <c r="G16" s="12">
-        <v>-49995</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G16" s="12"/>
       <c r="H16" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="9" t="s">
+      <c r="A17" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="12">
-        <v>-5</v>
-      </c>
-      <c r="G17" s="12">
-        <v>-5</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G17" s="12"/>
       <c r="H17" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -987,25 +941,23 @@
         <v>17</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F18" s="12">
-        <v>25</v>
-      </c>
-      <c r="G18" s="12">
-        <v>25</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="G18" s="12"/>
       <c r="H18" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1013,51 +965,47 @@
         <v>18</v>
       </c>
       <c r="B19" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="12">
+        <v>-2</v>
+      </c>
+      <c r="G19" s="12"/>
+      <c r="H19" s="11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F19" s="12">
-        <v>25</v>
-      </c>
-      <c r="G19" s="12">
-        <v>25</v>
-      </c>
-      <c r="H19" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B20" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>45</v>
-      </c>
       <c r="E20" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F20" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G20" s="12" t="s">
-        <v>29</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="F20" s="14">
+        <v>1.3</v>
+      </c>
+      <c r="G20" s="12"/>
       <c r="H20" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
@@ -1065,181 +1013,47 @@
         <v>20</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="F21" s="12">
-        <v>250000</v>
-      </c>
-      <c r="G21" s="12">
-        <v>250000</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G21" s="12"/>
       <c r="H21" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="12">
-        <v>0</v>
-      </c>
-      <c r="G22" s="12">
-        <v>0</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" s="12"/>
       <c r="H22" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="F23" s="12">
-        <v>1</v>
-      </c>
-      <c r="G23" s="12">
-        <v>1</v>
-      </c>
-      <c r="H23" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="F24" s="12">
-        <v>1</v>
-      </c>
-      <c r="G24" s="12">
-        <v>1</v>
-      </c>
-      <c r="H24" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B25" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E25" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="F25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="H25" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="F26" s="14">
-        <v>1E-4</v>
-      </c>
-      <c r="G26" s="14">
-        <v>1E-4</v>
-      </c>
-      <c r="H26" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="G27" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>